<commit_message>
run EVPI with (sensible) minimized optimization, Remove maximized optimization runs (not needed), shift sensitivity and Estimates to front
</commit_message>
<xml_diff>
--- a/Annual Gap Results.xlsx
+++ b/Annual Gap Results.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10212"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corywhitney/Dropbox/Contributions/17_Kenya_Fruit_Tree/kenya_fruit_trees/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76274BE3-F3CD-EF46-A8EE-0593B996E892}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34860" yWindow="10660" windowWidth="25600" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="740" yWindow="500" windowWidth="28180" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>Mean</t>
   </si>
@@ -61,13 +67,25 @@
   </si>
   <si>
     <t>Zinc (mg)</t>
+  </si>
+  <si>
+    <t>Mean(SD)</t>
+  </si>
+  <si>
+    <t>Average Difference (with trees)</t>
+  </si>
+  <si>
+    <t>Average daily difference</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="14"/>
       <color theme="1"/>
@@ -99,6 +117,28 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Garamond"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -117,7 +157,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -129,19 +169,29 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1"/>
+    <xf numFmtId="4" fontId="5" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="11" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
+    <cellStyle name="Comma" xfId="11" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -156,6 +206,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -480,272 +538,354 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:J13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16:I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="17" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.7109375" customWidth="1"/>
-    <col min="5" max="6" width="11.140625" customWidth="1"/>
-    <col min="7" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10" customWidth="1"/>
+    <col min="5" max="6" width="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="8.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:10">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="2:10" s="4" customFormat="1">
-      <c r="C5" s="2" t="s">
+    <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="2"/>
-    </row>
-    <row r="6" spans="2:10">
-      <c r="C6" s="1" t="s">
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="H6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="J6" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:10">
-      <c r="B7" s="1" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>-845.19</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="8">
         <v>263.88</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="8">
         <v>-584610</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="8">
         <v>-460170</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="8">
         <v>-1331200</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="8">
         <v>60582</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="8">
         <v>1169</v>
       </c>
-      <c r="J7">
+      <c r="J7" s="8">
         <v>2218</v>
       </c>
     </row>
-    <row r="8" spans="2:10">
-      <c r="B8" s="1" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>-332.15</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="8">
         <v>759.39</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="8">
         <v>341070</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="8">
         <v>364270</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="8">
         <v>58871</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="8">
         <v>204060</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="8">
         <v>1423.7</v>
       </c>
-      <c r="J8">
+      <c r="J8" s="8">
         <v>2299</v>
       </c>
     </row>
-    <row r="9" spans="2:10">
-      <c r="B9" s="1" t="s">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B9" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="8">
         <v>4636.7</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="8">
         <v>5273.9</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="8">
         <v>2845100</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="8">
         <v>2749200</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="8">
         <v>4320400</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="8">
         <v>1379300</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="8">
         <v>2173.4</v>
       </c>
-      <c r="J9">
+      <c r="J9" s="8">
         <v>1264.5999999999999</v>
       </c>
     </row>
-    <row r="10" spans="2:10">
-      <c r="B10" s="1" t="s">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="8">
         <v>21499000</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="8">
         <v>27814000</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="8">
         <v>8094600000000</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10" s="8">
         <v>7558300000000</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="8">
         <v>18666000000000</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="8">
         <v>1902500000000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="8">
         <v>4723700</v>
       </c>
-      <c r="J10">
+      <c r="J10" s="8">
         <v>1599300</v>
       </c>
     </row>
-    <row r="11" spans="2:10">
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="8">
         <v>-2961.3</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="8">
         <v>-2107.8000000000002</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="8">
         <v>-50495</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="8">
         <v>-17546</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="8">
         <v>-50625</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="8">
         <v>32576</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="8">
         <v>223.47</v>
       </c>
-      <c r="J11">
+      <c r="J11" s="8">
         <v>1263.7</v>
       </c>
     </row>
-    <row r="12" spans="2:10">
-      <c r="B12" s="1" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B12" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="8">
         <v>2005.7</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="8">
         <v>3557.6</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="8">
         <v>712510</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="8">
         <v>727770</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="8">
         <v>425800</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="8">
         <v>602030</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="8">
         <v>2572.5</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="8">
         <v>3207.8</v>
       </c>
     </row>
-    <row r="13" spans="2:10">
-      <c r="B13" s="1" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="7">
         <v>2.4015000000000002E-2</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="7">
         <v>0.84797999999999996</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="8">
         <v>25.422000000000001</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="8">
         <v>25.724</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="8">
         <v>859.16</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="8">
         <v>94.343999999999994</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="7">
         <v>5.7175000000000004E-3</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="7">
         <v>7.7378000000000004E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="str">
+        <f>C7&amp;"("&amp;C8&amp;")"</f>
+        <v>-845.19(-332.15)</v>
+      </c>
+      <c r="D15" t="str">
+        <f>D7&amp;"("&amp;D8&amp;")"</f>
+        <v>263.88(759.39)</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" ref="E15:J15" si="0">E7&amp;"("&amp;E8&amp;")"</f>
+        <v>-584610(341070)</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>-460170(364270)</v>
+      </c>
+      <c r="G15" t="str">
+        <f t="shared" si="0"/>
+        <v>-1331200(58871)</v>
+      </c>
+      <c r="H15" t="str">
+        <f t="shared" si="0"/>
+        <v>60582(204060)</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>1169(1423.7)</v>
+      </c>
+      <c r="J15" t="str">
+        <f t="shared" si="0"/>
+        <v>2218(2299)</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B16" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="9">
+        <f>C8-D8</f>
+        <v>-1091.54</v>
+      </c>
+      <c r="E16" s="9">
+        <f>E8-F8</f>
+        <v>-23200</v>
+      </c>
+      <c r="G16" s="9">
+        <f>G8-H8</f>
+        <v>-145189</v>
+      </c>
+      <c r="I16" s="9">
+        <f>I8-J8</f>
+        <v>-875.3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="10">
+        <f>C16/365</f>
+        <v>-2.9905205479452053</v>
+      </c>
+      <c r="E17" s="10">
+        <f>E16/365</f>
+        <v>-63.561643835616437</v>
+      </c>
+      <c r="G17" s="10">
+        <f>G16/365</f>
+        <v>-397.77808219178081</v>
+      </c>
+      <c r="I17" s="10">
+        <f>I16/365</f>
+        <v>-2.3980821917808219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modify and move results file
</commit_message>
<xml_diff>
--- a/Annual Gap Results.xlsx
+++ b/Annual Gap Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corywhitney/Dropbox/Contributions/17_Kenya_Fruit_Tree/kenya_fruit_trees/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76274BE3-F3CD-EF46-A8EE-0593B996E892}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86057DE9-1029-8E4E-A041-00D0D8D65960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="740" yWindow="500" windowWidth="28180" windowHeight="21900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -542,7 +542,7 @@
   <dimension ref="A4:J17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16:I17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>

</xml_diff>